<commit_message>
convert code to use openpyxl module instead
</commit_message>
<xml_diff>
--- a/HistoryReport.xlsx
+++ b/HistoryReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OneDrive - McGill University\Programming\screentime_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{18CAA01D-4F4F-4330-8F29-5C902AFA30C4}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5B4CAADA-2FC8-46F3-B44F-6B3FF4E218D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2CB47F07-EC7D-488E-B9BD-54EC2A300874}"/>
   </bookViews>
@@ -4629,23 +4629,27 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="9.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C1" t="s">
         <v>276</v>
       </c>
       <c r="D1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E1" t="s">
         <v>278</v>
@@ -4659,13 +4663,13 @@
         <v>280</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>2020</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2">
-        <v>2020</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -4676,6 +4680,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
comment out code that is not needed if I delete sheets with added data at the end of the program, add notFriday exception, make TODO list for next time
</commit_message>
<xml_diff>
--- a/HistoryReport.xlsx
+++ b/HistoryReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OneDrive - McGill University\Programming\screentime_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5B4CAADA-2FC8-46F3-B44F-6B3FF4E218D4}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7593FECE-3D2C-4B30-BD16-39C6E9EEEBFF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2CB47F07-EC7D-488E-B9BD-54EC2A300874}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="280">
   <si>
     <t>Saturday</t>
   </si>
@@ -873,9 +873,6 @@
   </si>
   <si>
     <t>Total_time</t>
-  </si>
-  <si>
-    <t>Su</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1250,7 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4626,10 +4623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3DB112-434C-405A-A76E-473F6707B8E1}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4656,26 +4653,6 @@
       </c>
       <c r="F1" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add intToExcelCol function, not perfect yet, extract column of app names from sheet to add col names to Data sheet, cannot add to Excel sheet yet
</commit_message>
<xml_diff>
--- a/HistoryReport.xlsx
+++ b/HistoryReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OneDrive - McGill University\Programming\screentime_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7593FECE-3D2C-4B30-BD16-39C6E9EEEBFF}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{026C6D53-E129-49BC-9242-62128D2A06FB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2CB47F07-EC7D-488E-B9BD-54EC2A300874}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="283">
   <si>
     <t>Saturday</t>
   </si>
@@ -873,6 +873,15 @@
   </si>
   <si>
     <t>Total_time</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -4623,10 +4632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3DB112-434C-405A-A76E-473F6707B8E1}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="A2:F2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4635,7 +4644,7 @@
     <col min="6" max="6" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>275</v>
       </c>
@@ -4653,6 +4662,15 @@
       </c>
       <c r="F1" t="s">
         <v>279</v>
+      </c>
+      <c r="G1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manually add app names to Data sheet
</commit_message>
<xml_diff>
--- a/HistoryReport.xlsx
+++ b/HistoryReport.xlsx
@@ -5,18 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OneDrive - McGill University\Programming\screentime_tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/aaron_lohner_mail_mcgill_ca/Documents/Programming/screentime_tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{026C6D53-E129-49BC-9242-62128D2A06FB}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{9203DA46-3BDC-4157-A8B5-FFCFF2CFA0E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{811E81CA-D1B1-473E-8C9E-91FD62FA7AD1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2CB47F07-EC7D-488E-B9BD-54EC2A300874}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{2CB47F07-EC7D-488E-B9BD-54EC2A300874}"/>
   </bookViews>
   <sheets>
     <sheet name="03-07-2020_20-22-08" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="3" r:id="rId2"/>
-    <sheet name="Pivot" sheetId="2" r:id="rId3"/>
+    <sheet name="Categories" sheetId="4" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Pivot" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="app_names">Data!$J$2:$DS$2</definedName>
+    <definedName name="time_info">Data!$A$2:$D$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="286">
   <si>
     <t>Saturday</t>
   </si>
@@ -872,16 +877,25 @@
     <t>Unlocks</t>
   </si>
   <si>
-    <t>Total_time</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>f</t>
+    <t>By category</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Social media</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Dating</t>
+  </si>
+  <si>
+    <t>app_names</t>
+  </si>
+  <si>
+    <t>time_info</t>
   </si>
 </sst>
 </file>
@@ -923,9 +937,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -935,13 +958,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,11 +1284,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB19DA0-D03C-4C81-8CD1-C7AF22A271F7}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A112" sqref="A111:A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
@@ -4631,46 +4660,985 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3DB112-434C-405A-A76E-473F6707B8E1}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16294A82-6D4C-4D24-AA57-2333CC0132CB}">
+  <dimension ref="A1:DZ116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" t="s">
-        <v>282</v>
+    <row r="1" spans="1:130" x14ac:dyDescent="0.35">
+      <c r="A1" t="e">
+        <f>tr</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B1" t="str">
+        <f t="array" ref="B1:DZ1">TRANSPOSE(A2:A115)</f>
+        <v>One UI Home</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Reminder</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Photos</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Facebook</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Messenger</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Instagram</v>
+      </c>
+      <c r="H1" t="str">
+        <v>LinkedIn</v>
+      </c>
+      <c r="I1" t="str">
+        <v>YouTube</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Outlook</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Samsung Notes</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Weather Network</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Netflix</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Clock</v>
+      </c>
+      <c r="P1" t="str">
+        <v>StayFree</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Android System</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Excel</v>
+      </c>
+      <c r="S1" t="str">
+        <v>WhatsApp</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Contacts</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Call</v>
+      </c>
+      <c r="W1" t="str">
+        <v>lichess</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Messages</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Snapchat</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>System UI</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Accessibility</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Token</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Google</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Chrome</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Samsung capture</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Spotify</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Samsung Internet</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Permission controller</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>OneDrive</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>Disney+</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Maps</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>Call settings</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Camera</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Gallery</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>Bixby Voice</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Calculator</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Weather</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Authenticator</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Shabbos Zmanim</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Google Play Store</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Gmail</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Calendar</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>Secure Folder</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>Slack</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Nectar</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Drive</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Docs</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>GroupMe</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>Lime</v>
+      </c>
+      <c r="BD1" t="str">
+        <v>Samsung Health</v>
+      </c>
+      <c r="BE1" t="str">
+        <v>Uber</v>
+      </c>
+      <c r="BF1" t="str">
+        <v>Amazon Shopping</v>
+      </c>
+      <c r="BG1" t="str">
+        <v>MyRogers</v>
+      </c>
+      <c r="BH1" t="str">
+        <v>PowerPoint</v>
+      </c>
+      <c r="BI1" t="str">
+        <v>Word</v>
+      </c>
+      <c r="BJ1" t="str">
+        <v>NHL</v>
+      </c>
+      <c r="BK1" t="str">
+        <v>Reminder</v>
+      </c>
+      <c r="BL1" t="str">
+        <v>Game Launcher</v>
+      </c>
+      <c r="BM1" t="str">
+        <v>My Files</v>
+      </c>
+      <c r="BN1" t="str">
+        <v>Galaxy Store</v>
+      </c>
+      <c r="BO1" t="str">
+        <v>Studentcare</v>
+      </c>
+      <c r="BP1" t="str">
+        <v>Passport</v>
+      </c>
+      <c r="BQ1" t="str">
+        <v>Bird</v>
+      </c>
+      <c r="BR1" t="str">
+        <v>Authenticator</v>
+      </c>
+      <c r="BS1" t="str">
+        <v>Chess</v>
+      </c>
+      <c r="BT1" t="str">
+        <v>Dictionary</v>
+      </c>
+      <c r="BU1" t="str">
+        <v>Eventbrite</v>
+      </c>
+      <c r="BV1" t="str">
+        <v>Wifi Analyzer</v>
+      </c>
+      <c r="BW1" t="str">
+        <v>Gett</v>
+      </c>
+      <c r="BX1" t="str">
+        <v>Translate</v>
+      </c>
+      <c r="BY1" t="str">
+        <v>Earth</v>
+      </c>
+      <c r="BZ1" t="str">
+        <v>IMDb</v>
+      </c>
+      <c r="CA1" t="str">
+        <v>ClearScanner</v>
+      </c>
+      <c r="CB1" t="str">
+        <v>Insta Downloader</v>
+      </c>
+      <c r="CC1" t="str">
+        <v>Smart Siddur</v>
+      </c>
+      <c r="CD1" t="str">
+        <v>Le Conjugueur</v>
+      </c>
+      <c r="CE1" t="str">
+        <v>McGill</v>
+      </c>
+      <c r="CF1" t="str">
+        <v>Israel Railways</v>
+      </c>
+      <c r="CG1" t="str">
+        <v>TI-36</v>
+      </c>
+      <c r="CH1" t="str">
+        <v>Find a set!</v>
+      </c>
+      <c r="CI1" t="str">
+        <v>Backgrounds</v>
+      </c>
+      <c r="CJ1" t="str">
+        <v>King's Mobile</v>
+      </c>
+      <c r="CK1" t="str">
+        <v>Ultimate VPN</v>
+      </c>
+      <c r="CL1" t="str">
+        <v>Wi-Fi</v>
+      </c>
+      <c r="CM1" t="str">
+        <v>Poll Everywhere</v>
+      </c>
+      <c r="CN1" t="str">
+        <v>myAppointment</v>
+      </c>
+      <c r="CO1" t="str">
+        <v>Video</v>
+      </c>
+      <c r="CP1" t="str">
+        <v>Voice Recorder</v>
+      </c>
+      <c r="CQ1" t="str">
+        <v>Smart Switch</v>
+      </c>
+      <c r="CR1" t="str">
+        <v>JSwipe</v>
+      </c>
+      <c r="CS1" t="str">
+        <v>Reverso Context</v>
+      </c>
+      <c r="CT1" t="str">
+        <v>TD (Canada)</v>
+      </c>
+      <c r="CU1" t="str">
+        <v>Transit</v>
+      </c>
+      <c r="CV1" t="str">
+        <v>Microsoft SwiftKey Keyboard</v>
+      </c>
+      <c r="CW1" t="str">
+        <v>Moovit</v>
+      </c>
+      <c r="CX1" t="str">
+        <v>TurningPoint</v>
+      </c>
+      <c r="CY1" t="str">
+        <v>Uber Driver</v>
+      </c>
+      <c r="CZ1" t="str">
+        <v>Click Counter</v>
+      </c>
+      <c r="DA1" t="str">
+        <v>Waze</v>
+      </c>
+      <c r="DB1" t="str">
+        <v>Poker Chip Counter</v>
+      </c>
+      <c r="DC1" t="str">
+        <v>Ruler</v>
+      </c>
+      <c r="DD1" t="str">
+        <v>Circuit</v>
+      </c>
+      <c r="DE1" t="str">
+        <v>Headphones</v>
+      </c>
+      <c r="DF1" t="str">
+        <v>Screen Time</v>
+      </c>
+      <c r="DG1" t="str">
+        <v>White Noise Generator</v>
+      </c>
+      <c r="DH1" t="str">
+        <v>FindTheSets</v>
+      </c>
+      <c r="DI1" t="str">
+        <v>Kahoot!</v>
+      </c>
+      <c r="DJ1" t="str">
+        <v>P$ Service Mobile</v>
+      </c>
+      <c r="DK1" t="str">
+        <v>Zoom</v>
+      </c>
+      <c r="DL1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DM1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DN1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DO1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DP1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DQ1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DR1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DS1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DT1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DU1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DV1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DW1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DX1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DY1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="DZ1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:130" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4680,6 +5648,410 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3DB112-434C-405A-A76E-473F6707B8E1}">
+  <dimension ref="A1:DS2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="6" width="9.36328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.1796875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:123" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:123" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" t="s">
+        <v>98</v>
+      </c>
+      <c r="W2" t="s">
+        <v>104</v>
+      </c>
+      <c r="X2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>194</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>199</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>201</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>207</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>208</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>210</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>215</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>216</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>217</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>219</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>220</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>194</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>221</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>222</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>223</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>224</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>225</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>226</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>227</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>228</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>229</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>230</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>231</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>232</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>233</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>234</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>235</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>236</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>237</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>238</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>239</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>240</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>241</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>243</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>245</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>246</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>247</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>248</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>249</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>250</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>251</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>252</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>253</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>254</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>255</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>256</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>257</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>258</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>261</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>262</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>263</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>264</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BDB31-F292-44D5-8EA0-7CA643D17249}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4876,18 +6248,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4909,25 +6281,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA831DEC-15FE-4574-A35E-70E1E6FF35F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f1d3745-27f9-43a1-8c6d-94a33c637ef6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E23A4906-77BF-408A-995A-227391470A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA831DEC-15FE-4574-A35E-70E1E6FF35F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f1d3745-27f9-43a1-8c6d-94a33c637ef6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>